<commit_message>
Update with EA Peer Review edits
Reformatted and edited control #4 to retain 3 backups per ARS 3.1
</commit_message>
<xml_diff>
--- a/cms-ars-3.1-moderate-aws-rds-infrastructure-cis-overlay.xlsx
+++ b/cms-ars-3.1-moderate-aws-rds-infrastructure-cis-overlay.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhaynes/Documents/inspec/cms/cms-ars-3.1-moderate-aws-rds-infrastructure-cis-overlay/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\Greg\Overlay_Worksheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2DA751C4-1D3B-7F48-B809-4EFA8F3664A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5644A50D-D453-4599-901E-E10FA712AA2F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="33600" windowHeight="21000"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cms-ars-3.1-moderate-aws-rds-in" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="87" uniqueCount="76">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="87" uniqueCount="80">
   <si>
     <t>title</t>
   </si>
@@ -58,9 +58,6 @@
   recommended to add inbound security group rules that allow traffic for the
   specific database protocol and ports by referencing as source the security
   group associated with the App tier instances.</t>
-  </si>
-  <si>
-    <t>["IA-5(1)", "Rev_4"]</t>
   </si>
   <si>
     <t xml:space="preserve">Using the Amazon unified command line interface:
@@ -205,24 +202,6 @@
   </si>
   <si>
     <t>Ensure Relational Database Service backup retention policy is set.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Using the Amazon unified command line interface:
-  * Check if your application DB instances have a Backup Retention Period set (0
-  = there is no backup retention in place, 7 = there are 7 daily backups
-  retained):
-  aws rds describe-db-instances --filters
-  Name=tag:&lt;data_tier_tag&gt;,Values=&lt;data_tier_tag_value&gt; --query
-  'DBInstances[*].{BackupRetentionPeriod:BackupRetentionPeriod,
-  DBInstanceIdentifier:DBInstanceIdentifier}'
-  </t>
-  </si>
-  <si>
-    <t>Using the Amazon unified command line interface:
-  * Modify each DB instance with Backup Retention Period of 0, and set a desired
-  Backup Retention Period in days (recommended value = 7):
-  aws rds modify-db-instance --db-instance-identifier &lt;your_db_instance&gt;
-  --backup- retention-period &lt;backup_retention_period&gt;</t>
   </si>
   <si>
     <t>aws-rds-baseline-4</t>
@@ -410,9 +389,6 @@
   * PostgreSQL.</t>
   </si>
   <si>
-    <t>Provides a managed backup function of the RDS Database, it is possible to define the backup window and retention period of the backup. Each customer should have a retention policy set for the type of data being stored. Recommend setting this to at least 7. Possible values are from 0 to 35 days.</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Ensure a SNS topic is created for sending out notifications from RDS events.</t>
   </si>
   <si>
@@ -469,12 +445,219 @@
   MariaDB - TCP 3306
   Amazon Aurora DB - TCP 3306</t>
   </si>
+  <si>
+    <t>["SC-28", "Rev_4"]</t>
+  </si>
+  <si>
+    <t>["CM-6", "Rev_4"]</t>
+  </si>
+  <si>
+    <t>["CP-9", "Rev_4"]</t>
+  </si>
+  <si>
+    <t>["IR-6", "Rev_4"]</t>
+  </si>
+  <si>
+    <t>["SC-7", "Rev_4"]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Provides a managed backup function of the RDS Database, it is possible to define the backup window and retention period of the backup. Each customer should have a retention policy set for the type of data being stored. Recommend setting this to at least </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Possible values are from 0 to 35 days.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Using the Amazon unified command line interface:
+  * Check if your application DB instances have a Backup Retention Period set (</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">0
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  = there is no backup retention in place,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = there are</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> daily backups retained):
+  aws rds describe-db-instances --filters
+  Name=tag:&lt;data_tier_tag&gt;,Values=&lt;data_tier_tag_value&gt; --query
+  'DBInstances[*].{BackupRetentionPeriod:BackupRetentionPeriod,
+  DBInstanceIdentifier:DBInstanceIdentifier}'
+  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using the Amazon unified command line interface:
+  * Modify each DB instance with Backup Retention Period of 0, and set a desired
+  Backup Retention Period in days (recommended value = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>):
+  aws rds modify-db-instance --db-instance-identifier &lt;your_db_instance&gt;
+  --backup- retention-period &lt;backup_retention_period&gt;</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,8 +792,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -790,8 +1006,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <start/>
       <end/>
@@ -906,6 +1128,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <start style="thin">
+        <color indexed="64"/>
+      </start>
+      <end style="thin">
+        <color indexed="64"/>
+      </end>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -951,18 +1188,33 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="10" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1319,379 +1571,398 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="34.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="53.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="54.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="60" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="17.296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.046875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="7.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.09765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.84765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="57.84765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="10.84765625" style="1"/>
+    <col min="10" max="10" width="18.34765625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.84765625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.6">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:10" ht="249.6" x14ac:dyDescent="0.6">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="312" x14ac:dyDescent="0.6">
+      <c r="A4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="234" x14ac:dyDescent="0.6">
+      <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" spans="1:10" ht="409.5" x14ac:dyDescent="0.6">
+      <c r="A6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4.2</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" spans="1:10" ht="374.4" x14ac:dyDescent="0.6">
+      <c r="A7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4.3</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="1:10" ht="374.4" x14ac:dyDescent="0.6">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="409.5" x14ac:dyDescent="0.6">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3">
+        <v>6.24</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" spans="1:10" ht="409.5" x14ac:dyDescent="0.6">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>50</v>
       </c>
+      <c r="C10" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="3">
+        <v>6.25</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="3"/>
     </row>
-    <row r="2" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="1">
+    <row r="11" spans="1:10" ht="374.4" x14ac:dyDescent="0.6">
+      <c r="A11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3">
         <v>0.3</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6.24</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="D11" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6.3</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="323" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="1">
+    <row r="12" spans="1:10" ht="374.4" x14ac:dyDescent="0.6">
+      <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="3">
         <v>0.3</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1">
-        <v>6.25</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="255" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4.3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="187" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="238" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3.6</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="255" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="1">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="255" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" s="1">
-        <v>3.8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="323" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="D12" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E12" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="1">
-        <v>4.2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1.4</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="G12" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="340" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E11" s="1">
+      <c r="H12" s="3">
         <v>6.34</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="323" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E12" s="1">
-        <v>6.3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="I12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N10">
+    <sortCondition ref="A2:A10"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>